<commit_message>
update CDC data added WHO data reports 1 through 40
</commit_message>
<xml_diff>
--- a/data/CDC_data.xlsx
+++ b/data/CDC_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauernd\Documents\R\workspace\COVID-19_epi_info\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66594FC2-95F4-4512-BFD1-6A4A02871D0C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD1A7CC-46D4-4EEC-B6EE-DD5CB3889ADF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2505" yWindow="195" windowWidth="14865" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1710" yWindow="825" windowWidth="14865" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CDC_data_as_of_14_Mar" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>25 mar data</t>
+  </si>
+  <si>
+    <t>26 mar data</t>
   </si>
 </sst>
 </file>
@@ -910,7 +913,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L76"/>
+  <dimension ref="A1:M76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -919,7 +922,7 @@
     <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -953,8 +956,11 @@
       <c r="L1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43842</v>
       </c>
@@ -988,8 +994,11 @@
       <c r="L2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43843</v>
       </c>
@@ -1023,8 +1032,11 @@
       <c r="L3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43844</v>
       </c>
@@ -1058,8 +1070,11 @@
       <c r="L4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43845</v>
       </c>
@@ -1093,8 +1108,11 @@
       <c r="L5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43846</v>
       </c>
@@ -1128,8 +1146,11 @@
       <c r="L6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43847</v>
       </c>
@@ -1163,8 +1184,11 @@
       <c r="L7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43848</v>
       </c>
@@ -1198,8 +1222,11 @@
       <c r="L8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43849</v>
       </c>
@@ -1233,8 +1260,11 @@
       <c r="L9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43850</v>
       </c>
@@ -1268,8 +1298,11 @@
       <c r="L10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43851</v>
       </c>
@@ -1303,8 +1336,11 @@
       <c r="L11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43852</v>
       </c>
@@ -1338,8 +1374,11 @@
       <c r="L12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43853</v>
       </c>
@@ -1373,8 +1412,11 @@
       <c r="L13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43854</v>
       </c>
@@ -1408,8 +1450,11 @@
       <c r="L14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43855</v>
       </c>
@@ -1443,8 +1488,11 @@
       <c r="L15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43856</v>
       </c>
@@ -1478,8 +1526,11 @@
       <c r="L16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43857</v>
       </c>
@@ -1513,8 +1564,11 @@
       <c r="L17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43858</v>
       </c>
@@ -1548,8 +1602,11 @@
       <c r="L18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43859</v>
       </c>
@@ -1583,8 +1640,11 @@
       <c r="L19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43860</v>
       </c>
@@ -1618,8 +1678,11 @@
       <c r="L20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43861</v>
       </c>
@@ -1653,8 +1716,11 @@
       <c r="L21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43862</v>
       </c>
@@ -1688,8 +1754,11 @@
       <c r="L22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43863</v>
       </c>
@@ -1723,8 +1792,11 @@
       <c r="L23">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43864</v>
       </c>
@@ -1758,8 +1830,11 @@
       <c r="L24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43865</v>
       </c>
@@ -1793,8 +1868,11 @@
       <c r="L25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43866</v>
       </c>
@@ -1828,8 +1906,11 @@
       <c r="L26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43867</v>
       </c>
@@ -1863,8 +1944,11 @@
       <c r="L27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43868</v>
       </c>
@@ -1898,8 +1982,11 @@
       <c r="L28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43869</v>
       </c>
@@ -1933,8 +2020,11 @@
       <c r="L29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43870</v>
       </c>
@@ -1968,8 +2058,11 @@
       <c r="L30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43871</v>
       </c>
@@ -2003,8 +2096,11 @@
       <c r="L31">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>43872</v>
       </c>
@@ -2038,8 +2134,11 @@
       <c r="L32">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43873</v>
       </c>
@@ -2073,8 +2172,11 @@
       <c r="L33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43874</v>
       </c>
@@ -2108,8 +2210,11 @@
       <c r="L34">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43875</v>
       </c>
@@ -2143,8 +2248,11 @@
       <c r="L35">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43876</v>
       </c>
@@ -2178,13 +2286,16 @@
       <c r="L36">
         <v>7</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M36">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43877</v>
       </c>
       <c r="B37">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -2213,8 +2324,11 @@
       <c r="L37">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>43878</v>
       </c>
@@ -2248,8 +2362,11 @@
       <c r="L38">
         <v>13</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M38">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>43879</v>
       </c>
@@ -2283,8 +2400,11 @@
       <c r="L39">
         <v>14</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M39">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>43880</v>
       </c>
@@ -2318,8 +2438,11 @@
       <c r="L40">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M40">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>43881</v>
       </c>
@@ -2353,8 +2476,11 @@
       <c r="L41">
         <v>12</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M41">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>43882</v>
       </c>
@@ -2388,8 +2514,11 @@
       <c r="L42">
         <v>23</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M42">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43883</v>
       </c>
@@ -2423,8 +2552,11 @@
       <c r="L43">
         <v>23</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M43">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43884</v>
       </c>
@@ -2458,8 +2590,11 @@
       <c r="L44">
         <v>23</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M44">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43885</v>
       </c>
@@ -2493,8 +2628,11 @@
       <c r="L45">
         <v>50</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M45">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>43886</v>
       </c>
@@ -2528,8 +2666,11 @@
       <c r="L46">
         <v>39</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M46">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>43887</v>
       </c>
@@ -2563,8 +2704,11 @@
       <c r="L47">
         <v>73</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M47">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>43888</v>
       </c>
@@ -2598,13 +2742,16 @@
       <c r="L48">
         <v>69</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M48">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>43889</v>
       </c>
       <c r="B49">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D49">
         <v>40</v>
@@ -2633,8 +2780,11 @@
       <c r="L49">
         <v>99</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M49">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>43890</v>
       </c>
@@ -2668,13 +2818,16 @@
       <c r="L50">
         <v>91</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M50">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>43891</v>
       </c>
       <c r="B51">
-        <v>173</v>
+        <v>273</v>
       </c>
       <c r="D51">
         <v>53</v>
@@ -2703,8 +2856,11 @@
       <c r="L51">
         <v>166</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M51">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>43892</v>
       </c>
@@ -2738,8 +2894,11 @@
       <c r="L52">
         <v>180</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M52">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>43893</v>
       </c>
@@ -2773,8 +2932,11 @@
       <c r="L53">
         <v>214</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M53">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>43894</v>
       </c>
@@ -2808,8 +2970,11 @@
       <c r="L54">
         <v>237</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M54">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>43895</v>
       </c>
@@ -2843,8 +3008,11 @@
       <c r="L55">
         <v>257</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M55">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>43896</v>
       </c>
@@ -2878,8 +3046,11 @@
       <c r="L56">
         <v>333</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M56">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>43897</v>
       </c>
@@ -2913,8 +3084,11 @@
       <c r="L57">
         <v>352</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M57">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>43898</v>
       </c>
@@ -2948,8 +3122,11 @@
       <c r="L58">
         <v>498</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M58">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>43899</v>
       </c>
@@ -2983,8 +3160,11 @@
       <c r="L59">
         <v>696</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M59">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>43900</v>
       </c>
@@ -3018,8 +3198,11 @@
       <c r="L60">
         <v>662</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M60">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>43901</v>
       </c>
@@ -3053,8 +3236,11 @@
       <c r="L61">
         <v>792</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M61">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>43902</v>
       </c>
@@ -3088,8 +3274,11 @@
       <c r="L62">
         <v>1055</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M62">
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>43903</v>
       </c>
@@ -3120,8 +3309,11 @@
       <c r="L63">
         <v>1113</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M63">
+        <v>1641</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>43904</v>
       </c>
@@ -3152,8 +3344,11 @@
       <c r="L64">
         <v>1058</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M64">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>43905</v>
       </c>
@@ -3184,8 +3379,11 @@
       <c r="L65">
         <v>1001</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M65">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>43906</v>
       </c>
@@ -3210,8 +3408,11 @@
       <c r="L66">
         <v>926</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M66">
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>43907</v>
       </c>
@@ -3236,13 +3437,16 @@
       <c r="L67">
         <v>467</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M67">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>43908</v>
       </c>
       <c r="B68">
-        <v>977</v>
+        <v>997</v>
       </c>
       <c r="G68">
         <v>0</v>
@@ -3262,8 +3466,11 @@
       <c r="L68">
         <v>302</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M68">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>43909</v>
       </c>
@@ -3285,8 +3492,11 @@
       <c r="L69">
         <v>187</v>
       </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M69">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>43910</v>
       </c>
@@ -3305,8 +3515,11 @@
       <c r="L70">
         <v>55</v>
       </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M70">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>43911</v>
       </c>
@@ -3322,8 +3535,11 @@
       <c r="L71">
         <v>13</v>
       </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M71">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>43912</v>
       </c>
@@ -3339,8 +3555,11 @@
       <c r="L72">
         <v>8</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M72">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>43913</v>
       </c>
@@ -3356,8 +3575,11 @@
       <c r="L73">
         <v>5</v>
       </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M73">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>43914</v>
       </c>
@@ -3370,8 +3592,11 @@
       <c r="L74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M74">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>43915</v>
       </c>
@@ -3381,12 +3606,18 @@
       <c r="L75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>43916</v>
       </c>
       <c r="B76">
+        <v>1</v>
+      </c>
+      <c r="M76">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
script updates and new CDC data
</commit_message>
<xml_diff>
--- a/data/CDC_data.xlsx
+++ b/data/CDC_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauernd\Documents\R\workspace\COVID-19_epi_info\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CC3B2C-7084-483B-A650-BEE4BCB6075D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64932106-0999-4D8B-8B08-409ED41A0F9E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5055" yWindow="1800" windowWidth="14025" windowHeight="7890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="945" yWindow="450" windowWidth="16665" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CDC_data_as_of_14_Mar" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>26 mar data</t>
+  </si>
+  <si>
+    <t>29 mar data</t>
   </si>
 </sst>
 </file>
@@ -913,10 +916,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M76"/>
+  <dimension ref="A1:N79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,7 +927,7 @@
     <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -961,8 +964,11 @@
       <c r="M1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43842</v>
       </c>
@@ -999,8 +1005,11 @@
       <c r="M2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43843</v>
       </c>
@@ -1037,13 +1046,16 @@
       <c r="M3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43844</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1075,8 +1087,11 @@
       <c r="M4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43845</v>
       </c>
@@ -1113,8 +1128,11 @@
       <c r="M5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43846</v>
       </c>
@@ -1151,8 +1169,11 @@
       <c r="M6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43847</v>
       </c>
@@ -1189,13 +1210,16 @@
       <c r="M7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43848</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1227,8 +1251,11 @@
       <c r="M8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43849</v>
       </c>
@@ -1265,8 +1292,11 @@
       <c r="M9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43850</v>
       </c>
@@ -1303,8 +1333,11 @@
       <c r="M10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43851</v>
       </c>
@@ -1341,13 +1374,16 @@
       <c r="M11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43852</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1379,8 +1415,11 @@
       <c r="M12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43853</v>
       </c>
@@ -1417,13 +1456,16 @@
       <c r="M13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43854</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1455,8 +1497,11 @@
       <c r="M14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43855</v>
       </c>
@@ -1493,8 +1538,11 @@
       <c r="M15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43856</v>
       </c>
@@ -1531,13 +1579,16 @@
       <c r="M16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43857</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1569,13 +1620,16 @@
       <c r="M17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43858</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18">
         <v>2</v>
@@ -1607,8 +1661,11 @@
       <c r="M18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43859</v>
       </c>
@@ -1645,8 +1702,11 @@
       <c r="M19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43860</v>
       </c>
@@ -1683,13 +1743,16 @@
       <c r="M20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43861</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1721,13 +1784,16 @@
       <c r="M21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43862</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1759,8 +1825,11 @@
       <c r="M22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43863</v>
       </c>
@@ -1797,8 +1866,11 @@
       <c r="M23">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43864</v>
       </c>
@@ -1835,8 +1907,11 @@
       <c r="M24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43865</v>
       </c>
@@ -1873,13 +1948,16 @@
       <c r="M25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43866</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -1911,8 +1989,11 @@
       <c r="M26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43867</v>
       </c>
@@ -1949,13 +2030,16 @@
       <c r="M27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43868</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -1987,13 +2071,16 @@
       <c r="M28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43869</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -2025,13 +2112,16 @@
       <c r="M29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43870</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -2063,8 +2153,11 @@
       <c r="M30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43871</v>
       </c>
@@ -2101,13 +2194,16 @@
       <c r="M31">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>43872</v>
       </c>
       <c r="B32">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -2139,13 +2235,16 @@
       <c r="M32">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43873</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -2177,13 +2276,16 @@
       <c r="M33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43874</v>
       </c>
       <c r="B34">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D34">
         <v>3</v>
@@ -2215,13 +2317,16 @@
       <c r="M34">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43875</v>
       </c>
       <c r="B35">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D35">
         <v>2</v>
@@ -2253,13 +2358,16 @@
       <c r="M35">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43876</v>
       </c>
       <c r="B36">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -2291,8 +2399,11 @@
       <c r="M36">
         <v>7</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N36">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43877</v>
       </c>
@@ -2329,13 +2440,16 @@
       <c r="M37">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>43878</v>
       </c>
       <c r="B38">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D38">
         <v>5</v>
@@ -2367,13 +2481,16 @@
       <c r="M38">
         <v>13</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N38">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>43879</v>
       </c>
       <c r="B39">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D39">
         <v>10</v>
@@ -2405,13 +2522,16 @@
       <c r="M39">
         <v>14</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N39">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>43880</v>
       </c>
       <c r="B40">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D40">
         <v>6</v>
@@ -2443,13 +2563,16 @@
       <c r="M40">
         <v>7</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N40">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>43881</v>
       </c>
       <c r="B41">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D41">
         <v>7</v>
@@ -2481,13 +2604,16 @@
       <c r="M41">
         <v>12</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N41">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>43882</v>
       </c>
       <c r="B42">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D42">
         <v>11</v>
@@ -2519,13 +2645,16 @@
       <c r="M42">
         <v>21</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N42">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43883</v>
       </c>
       <c r="B43">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D43">
         <v>14</v>
@@ -2557,13 +2686,16 @@
       <c r="M43">
         <v>20</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N43">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43884</v>
       </c>
       <c r="B44">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D44">
         <v>13</v>
@@ -2595,13 +2727,16 @@
       <c r="M44">
         <v>23</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N44">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43885</v>
       </c>
       <c r="B45">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="D45">
         <v>34</v>
@@ -2633,13 +2768,16 @@
       <c r="M45">
         <v>48</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N45">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>43886</v>
       </c>
       <c r="B46">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D46">
         <v>16</v>
@@ -2671,13 +2809,16 @@
       <c r="M46">
         <v>40</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N46">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>43887</v>
       </c>
       <c r="B47">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="D47">
         <v>30</v>
@@ -2709,13 +2850,16 @@
       <c r="M47">
         <v>74</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N47">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>43888</v>
       </c>
       <c r="B48">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D48">
         <v>19</v>
@@ -2747,13 +2891,16 @@
       <c r="M48">
         <v>71</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N48">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>43889</v>
       </c>
       <c r="B49">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="D49">
         <v>40</v>
@@ -2785,13 +2932,16 @@
       <c r="M49">
         <v>102</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N49">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>43890</v>
       </c>
       <c r="B50">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D50">
         <v>40</v>
@@ -2823,13 +2973,16 @@
       <c r="M50">
         <v>97</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N50">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>43891</v>
       </c>
       <c r="B51">
-        <v>173</v>
+        <v>208</v>
       </c>
       <c r="D51">
         <v>53</v>
@@ -2861,13 +3014,16 @@
       <c r="M51">
         <v>173</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N51">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>43892</v>
       </c>
       <c r="B52">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="D52">
         <v>51</v>
@@ -2899,13 +3055,16 @@
       <c r="M52">
         <v>188</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N52">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>43893</v>
       </c>
       <c r="B53">
-        <v>216</v>
+        <v>247</v>
       </c>
       <c r="D53">
         <v>48</v>
@@ -2937,13 +3096,16 @@
       <c r="M53">
         <v>216</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N53">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>43894</v>
       </c>
       <c r="B54">
-        <v>247</v>
+        <v>276</v>
       </c>
       <c r="D54">
         <v>58</v>
@@ -2975,13 +3137,16 @@
       <c r="M54">
         <v>247</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N54">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>43895</v>
       </c>
       <c r="B55">
-        <v>274</v>
+        <v>316</v>
       </c>
       <c r="D55">
         <v>74</v>
@@ -3013,13 +3178,16 @@
       <c r="M55">
         <v>274</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N55">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>43896</v>
       </c>
       <c r="B56">
-        <v>365</v>
+        <v>408</v>
       </c>
       <c r="D56">
         <v>43</v>
@@ -3051,13 +3219,16 @@
       <c r="M56">
         <v>365</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N56">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>43897</v>
       </c>
       <c r="B57">
-        <v>385</v>
+        <v>418</v>
       </c>
       <c r="D57">
         <v>79</v>
@@ -3089,13 +3260,16 @@
       <c r="M57">
         <v>385</v>
       </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N57">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>43898</v>
       </c>
       <c r="B58">
-        <v>548</v>
+        <v>611</v>
       </c>
       <c r="D58">
         <v>46</v>
@@ -3127,13 +3301,16 @@
       <c r="M58">
         <v>548</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N58">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>43899</v>
       </c>
       <c r="B59">
-        <v>782</v>
+        <v>696</v>
       </c>
       <c r="D59">
         <v>50</v>
@@ -3165,13 +3342,16 @@
       <c r="M59">
         <v>782</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N59">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>43900</v>
       </c>
       <c r="B60">
-        <v>767</v>
+        <v>970</v>
       </c>
       <c r="D60">
         <v>15</v>
@@ -3203,13 +3383,16 @@
       <c r="M60">
         <v>767</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N60">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>43901</v>
       </c>
       <c r="B61">
-        <v>993</v>
+        <v>1267</v>
       </c>
       <c r="D61">
         <v>2</v>
@@ -3241,13 +3424,16 @@
       <c r="M61">
         <v>993</v>
       </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N61">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>43902</v>
       </c>
       <c r="B62">
-        <v>1341</v>
+        <v>1775</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -3279,13 +3465,16 @@
       <c r="M62">
         <v>1341</v>
       </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N62">
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>43903</v>
       </c>
       <c r="B63">
-        <v>1641</v>
+        <v>2256</v>
       </c>
       <c r="E63">
         <v>2</v>
@@ -3314,13 +3503,16 @@
       <c r="M63">
         <v>1641</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N63">
+        <v>1641</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>43904</v>
       </c>
       <c r="B64">
-        <v>1634</v>
+        <v>2401</v>
       </c>
       <c r="E64">
         <v>0</v>
@@ -3349,13 +3541,16 @@
       <c r="M64">
         <v>1634</v>
       </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N64">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>43905</v>
       </c>
       <c r="B65">
-        <v>1905</v>
+        <v>2880</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -3384,13 +3579,16 @@
       <c r="M65">
         <v>1905</v>
       </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A66" s="2">
+      <c r="N65">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A66" s="3">
         <v>43906</v>
       </c>
       <c r="B66">
-        <v>1880</v>
+        <v>3060</v>
       </c>
       <c r="G66">
         <v>2</v>
@@ -3413,13 +3611,16 @@
       <c r="M66">
         <v>1880</v>
       </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A67" s="2">
+      <c r="N66">
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A67" s="3">
         <v>43907</v>
       </c>
       <c r="B67">
-        <v>1246</v>
+        <v>2344</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -3442,13 +3643,16 @@
       <c r="M67">
         <v>1246</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A68" s="2">
+      <c r="N67">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A68" s="3">
         <v>43908</v>
       </c>
       <c r="B68">
-        <v>977</v>
+        <v>2195</v>
       </c>
       <c r="G68">
         <v>0</v>
@@ -3471,13 +3675,16 @@
       <c r="M68">
         <v>977</v>
       </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N68">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>43909</v>
       </c>
       <c r="B69">
-        <v>896</v>
+        <v>2639</v>
       </c>
       <c r="H69">
         <v>0</v>
@@ -3497,13 +3704,16 @@
       <c r="M69">
         <v>896</v>
       </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N69">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>43910</v>
       </c>
       <c r="B70">
-        <v>457</v>
+        <v>2236</v>
       </c>
       <c r="I70">
         <v>2</v>
@@ -3520,13 +3730,16 @@
       <c r="M70">
         <v>457</v>
       </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N70">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>43911</v>
       </c>
       <c r="B71">
-        <v>179</v>
+        <v>2248</v>
       </c>
       <c r="J71">
         <v>2</v>
@@ -3540,13 +3753,16 @@
       <c r="M71">
         <v>179</v>
       </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N71">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>43912</v>
       </c>
       <c r="B72">
-        <v>90</v>
+        <v>1541</v>
       </c>
       <c r="J72">
         <v>1</v>
@@ -3560,13 +3776,16 @@
       <c r="M72">
         <v>90</v>
       </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N72">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>43913</v>
       </c>
       <c r="B73">
-        <v>59</v>
+        <v>515</v>
       </c>
       <c r="J73">
         <v>0</v>
@@ -3580,13 +3799,16 @@
       <c r="M73">
         <v>59</v>
       </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N73">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>43914</v>
       </c>
       <c r="B74">
-        <v>7</v>
+        <v>201</v>
       </c>
       <c r="K74">
         <v>0</v>
@@ -3597,13 +3819,16 @@
       <c r="M74">
         <v>7</v>
       </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N74">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>43915</v>
       </c>
       <c r="B75">
-        <v>1</v>
+        <v>107</v>
       </c>
       <c r="L75">
         <v>0</v>
@@ -3611,16 +3836,46 @@
       <c r="M75">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>43916</v>
       </c>
       <c r="B76">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="M76">
         <v>1</v>
+      </c>
+      <c r="N76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B77">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>43918</v>
+      </c>
+      <c r="B78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>43919</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1 apr 20 update
</commit_message>
<xml_diff>
--- a/data/CDC_data.xlsx
+++ b/data/CDC_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauernd\Documents\R\workspace\COVID-19_epi_info\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64932106-0999-4D8B-8B08-409ED41A0F9E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2984D6-B140-453C-8042-2EDF96DDE5D6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="450" windowWidth="16665" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2520" yWindow="555" windowWidth="16665" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CDC_data_as_of_14_Mar" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>29 mar data</t>
+  </si>
+  <si>
+    <t>30 mar data</t>
   </si>
 </sst>
 </file>
@@ -916,10 +919,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N79"/>
+  <dimension ref="A1:O81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,7 +930,7 @@
     <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -967,8 +970,11 @@
       <c r="N1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43842</v>
       </c>
@@ -1008,8 +1014,11 @@
       <c r="N2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43843</v>
       </c>
@@ -1049,8 +1058,11 @@
       <c r="N3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43844</v>
       </c>
@@ -1090,8 +1102,11 @@
       <c r="N4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43845</v>
       </c>
@@ -1131,8 +1146,11 @@
       <c r="N5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43846</v>
       </c>
@@ -1172,8 +1190,11 @@
       <c r="N6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43847</v>
       </c>
@@ -1213,8 +1234,11 @@
       <c r="N7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43848</v>
       </c>
@@ -1254,8 +1278,11 @@
       <c r="N8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43849</v>
       </c>
@@ -1295,8 +1322,11 @@
       <c r="N9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43850</v>
       </c>
@@ -1336,8 +1366,11 @@
       <c r="N10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43851</v>
       </c>
@@ -1377,13 +1410,16 @@
       <c r="N11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43852</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1418,8 +1454,11 @@
       <c r="N12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43853</v>
       </c>
@@ -1459,8 +1498,11 @@
       <c r="N13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43854</v>
       </c>
@@ -1500,8 +1542,11 @@
       <c r="N14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43855</v>
       </c>
@@ -1541,8 +1586,11 @@
       <c r="N15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43856</v>
       </c>
@@ -1582,8 +1630,11 @@
       <c r="N16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43857</v>
       </c>
@@ -1623,8 +1674,11 @@
       <c r="N17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43858</v>
       </c>
@@ -1664,8 +1718,11 @@
       <c r="N18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43859</v>
       </c>
@@ -1705,8 +1762,11 @@
       <c r="N19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43860</v>
       </c>
@@ -1746,8 +1806,11 @@
       <c r="N20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43861</v>
       </c>
@@ -1787,13 +1850,16 @@
       <c r="N21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43862</v>
       </c>
       <c r="B22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1828,8 +1894,11 @@
       <c r="N22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43863</v>
       </c>
@@ -1869,8 +1938,11 @@
       <c r="N23">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43864</v>
       </c>
@@ -1910,8 +1982,11 @@
       <c r="N24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43865</v>
       </c>
@@ -1951,8 +2026,11 @@
       <c r="N25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43866</v>
       </c>
@@ -1992,8 +2070,11 @@
       <c r="N26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43867</v>
       </c>
@@ -2033,13 +2114,16 @@
       <c r="N27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43868</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -2074,13 +2158,16 @@
       <c r="N28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43869</v>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -2115,8 +2202,11 @@
       <c r="N29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43870</v>
       </c>
@@ -2156,8 +2246,11 @@
       <c r="N30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43871</v>
       </c>
@@ -2197,13 +2290,16 @@
       <c r="N31">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>43872</v>
       </c>
       <c r="B32">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -2238,13 +2334,16 @@
       <c r="N32">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43873</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -2279,8 +2378,11 @@
       <c r="N33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43874</v>
       </c>
@@ -2320,54 +2422,60 @@
       <c r="N34">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43875</v>
       </c>
       <c r="B35">
+        <v>7</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35">
+        <v>2</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>3</v>
+      </c>
+      <c r="I35">
+        <v>3</v>
+      </c>
+      <c r="J35">
+        <v>3</v>
+      </c>
+      <c r="K35">
+        <v>3</v>
+      </c>
+      <c r="L35">
+        <v>3</v>
+      </c>
+      <c r="M35">
+        <v>3</v>
+      </c>
+      <c r="N35">
+        <v>3</v>
+      </c>
+      <c r="O35">
         <v>5</v>
       </c>
-      <c r="D35">
-        <v>2</v>
-      </c>
-      <c r="E35">
-        <v>2</v>
-      </c>
-      <c r="F35">
-        <v>2</v>
-      </c>
-      <c r="G35">
-        <v>1</v>
-      </c>
-      <c r="H35">
-        <v>3</v>
-      </c>
-      <c r="I35">
-        <v>3</v>
-      </c>
-      <c r="J35">
-        <v>3</v>
-      </c>
-      <c r="K35">
-        <v>3</v>
-      </c>
-      <c r="L35">
-        <v>3</v>
-      </c>
-      <c r="M35">
-        <v>3</v>
-      </c>
-      <c r="N35">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43876</v>
       </c>
       <c r="B36">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -2402,13 +2510,16 @@
       <c r="N36">
         <v>7</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43877</v>
       </c>
       <c r="B37">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -2443,13 +2554,16 @@
       <c r="N37">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>43878</v>
       </c>
       <c r="B38">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D38">
         <v>5</v>
@@ -2484,13 +2598,16 @@
       <c r="N38">
         <v>13</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O38">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>43879</v>
       </c>
       <c r="B39">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D39">
         <v>10</v>
@@ -2525,13 +2642,16 @@
       <c r="N39">
         <v>14</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O39">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>43880</v>
       </c>
       <c r="B40">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D40">
         <v>6</v>
@@ -2566,13 +2686,16 @@
       <c r="N40">
         <v>7</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O40">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>43881</v>
       </c>
       <c r="B41">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D41">
         <v>7</v>
@@ -2607,13 +2730,16 @@
       <c r="N41">
         <v>12</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O41">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>43882</v>
       </c>
       <c r="B42">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="D42">
         <v>11</v>
@@ -2648,13 +2774,16 @@
       <c r="N42">
         <v>21</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O42">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43883</v>
       </c>
       <c r="B43">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D43">
         <v>14</v>
@@ -2689,13 +2818,16 @@
       <c r="N43">
         <v>20</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O43">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43884</v>
       </c>
       <c r="B44">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D44">
         <v>13</v>
@@ -2730,13 +2862,16 @@
       <c r="N44">
         <v>23</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O44">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43885</v>
       </c>
       <c r="B45">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="D45">
         <v>34</v>
@@ -2771,13 +2906,16 @@
       <c r="N45">
         <v>48</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O45">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>43886</v>
       </c>
       <c r="B46">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D46">
         <v>16</v>
@@ -2812,13 +2950,16 @@
       <c r="N46">
         <v>40</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>43887</v>
       </c>
       <c r="B47">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="D47">
         <v>30</v>
@@ -2853,13 +2994,16 @@
       <c r="N47">
         <v>74</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O47">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>43888</v>
       </c>
       <c r="B48">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="D48">
         <v>19</v>
@@ -2894,13 +3038,16 @@
       <c r="N48">
         <v>71</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O48">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>43889</v>
       </c>
       <c r="B49">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="D49">
         <v>40</v>
@@ -2935,13 +3082,16 @@
       <c r="N49">
         <v>102</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O49">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>43890</v>
       </c>
       <c r="B50">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="D50">
         <v>40</v>
@@ -2976,13 +3126,16 @@
       <c r="N50">
         <v>97</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O50">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>43891</v>
       </c>
       <c r="B51">
-        <v>208</v>
+        <v>251</v>
       </c>
       <c r="D51">
         <v>53</v>
@@ -3017,13 +3170,16 @@
       <c r="N51">
         <v>173</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O51">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>43892</v>
       </c>
       <c r="B52">
-        <v>204</v>
+        <v>245</v>
       </c>
       <c r="D52">
         <v>51</v>
@@ -3058,13 +3214,16 @@
       <c r="N52">
         <v>188</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O52">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>43893</v>
       </c>
       <c r="B53">
-        <v>247</v>
+        <v>285</v>
       </c>
       <c r="D53">
         <v>48</v>
@@ -3099,13 +3258,16 @@
       <c r="N53">
         <v>216</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O53">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>43894</v>
       </c>
       <c r="B54">
-        <v>276</v>
+        <v>322</v>
       </c>
       <c r="D54">
         <v>58</v>
@@ -3140,13 +3302,16 @@
       <c r="N54">
         <v>247</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O54">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>43895</v>
       </c>
       <c r="B55">
-        <v>316</v>
+        <v>378</v>
       </c>
       <c r="D55">
         <v>74</v>
@@ -3181,13 +3346,16 @@
       <c r="N55">
         <v>274</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O55">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>43896</v>
       </c>
       <c r="B56">
-        <v>408</v>
+        <v>479</v>
       </c>
       <c r="D56">
         <v>43</v>
@@ -3222,13 +3390,16 @@
       <c r="N56">
         <v>365</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O56">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>43897</v>
       </c>
       <c r="B57">
-        <v>418</v>
+        <v>501</v>
       </c>
       <c r="D57">
         <v>79</v>
@@ -3263,13 +3434,16 @@
       <c r="N57">
         <v>385</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O57">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>43898</v>
       </c>
       <c r="B58">
-        <v>611</v>
+        <v>736</v>
       </c>
       <c r="D58">
         <v>46</v>
@@ -3304,13 +3478,16 @@
       <c r="N58">
         <v>548</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O58">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>43899</v>
       </c>
       <c r="B59">
-        <v>696</v>
+        <v>1151</v>
       </c>
       <c r="D59">
         <v>50</v>
@@ -3345,13 +3522,16 @@
       <c r="N59">
         <v>782</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O59">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>43900</v>
       </c>
       <c r="B60">
-        <v>970</v>
+        <v>1206</v>
       </c>
       <c r="D60">
         <v>15</v>
@@ -3386,13 +3566,16 @@
       <c r="N60">
         <v>767</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O60">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>43901</v>
       </c>
       <c r="B61">
-        <v>1267</v>
+        <v>1581</v>
       </c>
       <c r="D61">
         <v>2</v>
@@ -3427,13 +3610,16 @@
       <c r="N61">
         <v>993</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O61">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>43902</v>
       </c>
       <c r="B62">
-        <v>1775</v>
+        <v>2105</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -3468,13 +3654,16 @@
       <c r="N62">
         <v>1341</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O62">
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>43903</v>
       </c>
       <c r="B63">
-        <v>2256</v>
+        <v>2778</v>
       </c>
       <c r="E63">
         <v>2</v>
@@ -3506,13 +3695,16 @@
       <c r="N63">
         <v>1641</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O63">
+        <v>2256</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>43904</v>
       </c>
       <c r="B64">
-        <v>2401</v>
+        <v>2924</v>
       </c>
       <c r="E64">
         <v>0</v>
@@ -3544,13 +3736,16 @@
       <c r="N64">
         <v>1634</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O64">
+        <v>2401</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>43905</v>
       </c>
       <c r="B65">
-        <v>2880</v>
+        <v>3531</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -3582,13 +3777,16 @@
       <c r="N65">
         <v>1905</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O65">
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>43906</v>
       </c>
       <c r="B66">
-        <v>3060</v>
+        <v>3903</v>
       </c>
       <c r="G66">
         <v>2</v>
@@ -3614,13 +3812,16 @@
       <c r="N66">
         <v>1880</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O66">
+        <v>3060</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>43907</v>
       </c>
       <c r="B67">
-        <v>2344</v>
+        <v>3162</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -3646,13 +3847,16 @@
       <c r="N67">
         <v>1246</v>
       </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O67">
+        <v>2344</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>43908</v>
       </c>
       <c r="B68">
-        <v>2195</v>
+        <v>3029</v>
       </c>
       <c r="G68">
         <v>0</v>
@@ -3678,13 +3882,16 @@
       <c r="N68">
         <v>977</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A69" s="2">
+      <c r="O68">
+        <v>2195</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A69" s="3">
         <v>43909</v>
       </c>
       <c r="B69">
-        <v>2639</v>
+        <v>3651</v>
       </c>
       <c r="H69">
         <v>0</v>
@@ -3707,13 +3914,16 @@
       <c r="N69">
         <v>896</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A70" s="2">
+      <c r="O69">
+        <v>2639</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A70" s="3">
         <v>43910</v>
       </c>
       <c r="B70">
-        <v>2236</v>
+        <v>3661</v>
       </c>
       <c r="I70">
         <v>2</v>
@@ -3733,13 +3943,16 @@
       <c r="N70">
         <v>457</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O70">
+        <v>2236</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>43911</v>
       </c>
       <c r="B71">
-        <v>2248</v>
+        <v>3252</v>
       </c>
       <c r="J71">
         <v>2</v>
@@ -3756,13 +3969,16 @@
       <c r="N71">
         <v>179</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O71">
+        <v>2248</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>43912</v>
       </c>
       <c r="B72">
-        <v>1541</v>
+        <v>2884</v>
       </c>
       <c r="J72">
         <v>1</v>
@@ -3779,13 +3995,16 @@
       <c r="N72">
         <v>90</v>
       </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O72">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>43913</v>
       </c>
       <c r="B73">
-        <v>515</v>
+        <v>2139</v>
       </c>
       <c r="J73">
         <v>0</v>
@@ -3802,13 +4021,16 @@
       <c r="N73">
         <v>59</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O73">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>43914</v>
       </c>
       <c r="B74">
-        <v>201</v>
+        <v>1279</v>
       </c>
       <c r="K74">
         <v>0</v>
@@ -3822,59 +4044,93 @@
       <c r="N74">
         <v>7</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O74">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>43915</v>
       </c>
       <c r="B75">
+        <v>843</v>
+      </c>
+      <c r="L75">
+        <v>0</v>
+      </c>
+      <c r="M75">
+        <v>1</v>
+      </c>
+      <c r="N75">
+        <v>1</v>
+      </c>
+      <c r="O75">
         <v>107</v>
       </c>
-      <c r="L75">
-        <v>0</v>
-      </c>
-      <c r="M75">
-        <v>1</v>
-      </c>
-      <c r="N75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>43916</v>
       </c>
       <c r="B76">
+        <v>510</v>
+      </c>
+      <c r="M76">
+        <v>1</v>
+      </c>
+      <c r="N76">
+        <v>1</v>
+      </c>
+      <c r="O76">
         <v>37</v>
       </c>
-      <c r="M76">
-        <v>1</v>
-      </c>
-      <c r="N76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>43917</v>
       </c>
       <c r="B77">
+        <v>245</v>
+      </c>
+      <c r="O77">
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>43918</v>
       </c>
       <c r="B78">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="O78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>43919</v>
       </c>
       <c r="B79">
+        <v>33</v>
+      </c>
+      <c r="O79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>43920</v>
+      </c>
+      <c r="B80">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>43921</v>
+      </c>
+      <c r="B81">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update cdc and who data
</commit_message>
<xml_diff>
--- a/data/CDC_data.xlsx
+++ b/data/CDC_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauernd\Documents\R\workspace\COVID-19_epi_info\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF28009A-6FF2-4C50-8DE0-C58680C2F779}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DBA819-C908-40DE-BD9D-B72D77B1A7D0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1335" yWindow="330" windowWidth="16665" windowHeight="10845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2595" yWindow="330" windowWidth="15660" windowHeight="10845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CDC_data_as_of_14_Mar" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>2 apr data</t>
+  </si>
+  <si>
+    <t>3 apr data</t>
   </si>
 </sst>
 </file>
@@ -925,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q83"/>
+  <dimension ref="A1:R87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,7 +939,7 @@
     <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -985,8 +988,11 @@
       <c r="Q1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43842</v>
       </c>
@@ -1035,8 +1041,11 @@
       <c r="Q2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43843</v>
       </c>
@@ -1085,8 +1094,11 @@
       <c r="Q3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43844</v>
       </c>
@@ -1135,13 +1147,16 @@
       <c r="Q4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43845</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1185,13 +1200,16 @@
       <c r="Q5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43846</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1235,8 +1253,11 @@
       <c r="Q6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43847</v>
       </c>
@@ -1285,8 +1306,11 @@
       <c r="Q7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43848</v>
       </c>
@@ -1335,8 +1359,11 @@
       <c r="Q8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43849</v>
       </c>
@@ -1385,8 +1412,11 @@
       <c r="Q9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43850</v>
       </c>
@@ -1435,8 +1465,11 @@
       <c r="Q10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43851</v>
       </c>
@@ -1485,8 +1518,11 @@
       <c r="Q11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43852</v>
       </c>
@@ -1535,8 +1571,11 @@
       <c r="Q12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43853</v>
       </c>
@@ -1585,8 +1624,11 @@
       <c r="Q13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43854</v>
       </c>
@@ -1635,13 +1677,16 @@
       <c r="Q14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43855</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15">
         <v>3</v>
@@ -1685,8 +1730,11 @@
       <c r="Q15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43856</v>
       </c>
@@ -1735,8 +1783,11 @@
       <c r="Q16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43857</v>
       </c>
@@ -1785,8 +1836,11 @@
       <c r="Q17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43858</v>
       </c>
@@ -1835,13 +1889,16 @@
       <c r="Q18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43859</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1885,58 +1942,64 @@
       <c r="Q19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43860</v>
       </c>
       <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>2</v>
+      </c>
+      <c r="N20">
+        <v>2</v>
+      </c>
+      <c r="O20">
+        <v>2</v>
+      </c>
+      <c r="P20">
+        <v>2</v>
+      </c>
+      <c r="Q20">
+        <v>3</v>
+      </c>
+      <c r="R20">
         <v>4</v>
       </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-      <c r="I20">
-        <v>1</v>
-      </c>
-      <c r="J20">
-        <v>1</v>
-      </c>
-      <c r="K20">
-        <v>1</v>
-      </c>
-      <c r="L20">
-        <v>1</v>
-      </c>
-      <c r="M20">
-        <v>2</v>
-      </c>
-      <c r="N20">
-        <v>2</v>
-      </c>
-      <c r="O20">
-        <v>2</v>
-      </c>
-      <c r="P20">
-        <v>2</v>
-      </c>
-      <c r="Q20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43861</v>
       </c>
@@ -1985,8 +2048,11 @@
       <c r="Q21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43862</v>
       </c>
@@ -2035,8 +2101,11 @@
       <c r="Q22">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43863</v>
       </c>
@@ -2085,8 +2154,11 @@
       <c r="Q23">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43864</v>
       </c>
@@ -2135,8 +2207,11 @@
       <c r="Q24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43865</v>
       </c>
@@ -2185,8 +2260,11 @@
       <c r="Q25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43866</v>
       </c>
@@ -2235,8 +2313,11 @@
       <c r="Q26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43867</v>
       </c>
@@ -2285,13 +2366,16 @@
       <c r="Q27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43868</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -2335,8 +2419,11 @@
       <c r="Q28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43869</v>
       </c>
@@ -2385,13 +2472,16 @@
       <c r="Q29">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43870</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -2435,13 +2525,16 @@
       <c r="Q30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43871</v>
       </c>
       <c r="B31">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D31">
         <v>3</v>
@@ -2485,8 +2578,11 @@
       <c r="Q31">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>43872</v>
       </c>
@@ -2535,58 +2631,64 @@
       <c r="Q32">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R32">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43873</v>
       </c>
       <c r="B33">
+        <v>6</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <v>1</v>
+      </c>
+      <c r="P33">
+        <v>2</v>
+      </c>
+      <c r="Q33">
+        <v>2</v>
+      </c>
+      <c r="R33">
         <v>5</v>
       </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-      <c r="F33">
-        <v>1</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="I33">
-        <v>0</v>
-      </c>
-      <c r="J33">
-        <v>0</v>
-      </c>
-      <c r="K33">
-        <v>0</v>
-      </c>
-      <c r="L33">
-        <v>0</v>
-      </c>
-      <c r="M33">
-        <v>0</v>
-      </c>
-      <c r="N33">
-        <v>0</v>
-      </c>
-      <c r="O33">
-        <v>1</v>
-      </c>
-      <c r="P33">
-        <v>2</v>
-      </c>
-      <c r="Q33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43874</v>
       </c>
@@ -2635,13 +2737,16 @@
       <c r="Q34">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43875</v>
       </c>
       <c r="B35">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D35">
         <v>2</v>
@@ -2685,13 +2790,16 @@
       <c r="Q35">
         <v>7</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43876</v>
       </c>
       <c r="B36">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -2735,8 +2843,11 @@
       <c r="Q36">
         <v>10</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R36">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43877</v>
       </c>
@@ -2785,8 +2896,11 @@
       <c r="Q37">
         <v>6</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R37">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>43878</v>
       </c>
@@ -2835,13 +2949,16 @@
       <c r="Q38">
         <v>16</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R38">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>43879</v>
       </c>
       <c r="B39">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D39">
         <v>10</v>
@@ -2885,13 +3002,16 @@
       <c r="Q39">
         <v>18</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R39">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>43880</v>
       </c>
       <c r="B40">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D40">
         <v>6</v>
@@ -2935,13 +3055,16 @@
       <c r="Q40">
         <v>11</v>
       </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R40">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>43881</v>
       </c>
       <c r="B41">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D41">
         <v>7</v>
@@ -2985,13 +3108,16 @@
       <c r="Q41">
         <v>20</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R41">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>43882</v>
       </c>
       <c r="B42">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D42">
         <v>11</v>
@@ -3035,13 +3161,16 @@
       <c r="Q42">
         <v>31</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R42">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43883</v>
       </c>
       <c r="B43">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D43">
         <v>14</v>
@@ -3085,13 +3214,16 @@
       <c r="Q43">
         <v>38</v>
       </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R43">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43884</v>
       </c>
       <c r="B44">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D44">
         <v>13</v>
@@ -3135,13 +3267,16 @@
       <c r="Q44">
         <v>33</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R44">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43885</v>
       </c>
       <c r="B45">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D45">
         <v>34</v>
@@ -3185,13 +3320,16 @@
       <c r="Q45">
         <v>67</v>
       </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R45">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>43886</v>
       </c>
       <c r="B46">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D46">
         <v>16</v>
@@ -3235,13 +3373,16 @@
       <c r="Q46">
         <v>51</v>
       </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R46">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>43887</v>
       </c>
       <c r="B47">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D47">
         <v>30</v>
@@ -3285,13 +3426,16 @@
       <c r="Q47">
         <v>93</v>
       </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R47">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>43888</v>
       </c>
       <c r="B48">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="D48">
         <v>19</v>
@@ -3335,13 +3479,16 @@
       <c r="Q48">
         <v>85</v>
       </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R48">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>43889</v>
       </c>
       <c r="B49">
-        <v>137</v>
+        <v>152</v>
       </c>
       <c r="D49">
         <v>40</v>
@@ -3385,13 +3532,16 @@
       <c r="Q49">
         <v>129</v>
       </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R49">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>43890</v>
       </c>
       <c r="B50">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="D50">
         <v>40</v>
@@ -3435,13 +3585,16 @@
       <c r="Q50">
         <v>117</v>
       </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R50">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>43891</v>
       </c>
       <c r="B51">
-        <v>272</v>
+        <v>307</v>
       </c>
       <c r="D51">
         <v>53</v>
@@ -3485,13 +3638,16 @@
       <c r="Q51">
         <v>256</v>
       </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R51">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>43892</v>
       </c>
       <c r="B52">
-        <v>273</v>
+        <v>300</v>
       </c>
       <c r="D52">
         <v>51</v>
@@ -3535,13 +3691,16 @@
       <c r="Q52">
         <v>254</v>
       </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R52">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>43893</v>
       </c>
       <c r="B53">
-        <v>317</v>
+        <v>341</v>
       </c>
       <c r="D53">
         <v>48</v>
@@ -3585,13 +3744,16 @@
       <c r="Q53">
         <v>294</v>
       </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R53">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>43894</v>
       </c>
       <c r="B54">
-        <v>351</v>
+        <v>386</v>
       </c>
       <c r="D54">
         <v>58</v>
@@ -3635,13 +3797,16 @@
       <c r="Q54">
         <v>327</v>
       </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R54">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>43895</v>
       </c>
       <c r="B55">
-        <v>415</v>
+        <v>461</v>
       </c>
       <c r="D55">
         <v>74</v>
@@ -3685,13 +3850,16 @@
       <c r="Q55">
         <v>384</v>
       </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R55">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>43896</v>
       </c>
       <c r="B56">
-        <v>520</v>
+        <v>583</v>
       </c>
       <c r="D56">
         <v>43</v>
@@ -3735,13 +3903,16 @@
       <c r="Q56">
         <v>496</v>
       </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R56">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>43897</v>
       </c>
       <c r="B57">
-        <v>571</v>
+        <v>650</v>
       </c>
       <c r="D57">
         <v>79</v>
@@ -3785,13 +3956,16 @@
       <c r="Q57">
         <v>512</v>
       </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R57">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>43898</v>
       </c>
       <c r="B58">
-        <v>803</v>
+        <v>902</v>
       </c>
       <c r="D58">
         <v>46</v>
@@ -3835,13 +4009,16 @@
       <c r="Q58">
         <v>757</v>
       </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R58">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>43899</v>
       </c>
       <c r="B59">
-        <v>1288</v>
+        <v>1487</v>
       </c>
       <c r="D59">
         <v>50</v>
@@ -3885,13 +4062,16 @@
       <c r="Q59">
         <v>1188</v>
       </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R59">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>43900</v>
       </c>
       <c r="B60">
-        <v>1387</v>
+        <v>1618</v>
       </c>
       <c r="D60">
         <v>15</v>
@@ -3935,13 +4115,16 @@
       <c r="Q60">
         <v>1265</v>
       </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R60">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>43901</v>
       </c>
       <c r="B61">
-        <v>1775</v>
+        <v>2033</v>
       </c>
       <c r="D61">
         <v>2</v>
@@ -3985,13 +4168,16 @@
       <c r="Q61">
         <v>1637</v>
       </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R61">
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>43902</v>
       </c>
       <c r="B62">
-        <v>2351</v>
+        <v>2747</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -4035,13 +4221,16 @@
       <c r="Q62">
         <v>2198</v>
       </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R62">
+        <v>2351</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>43903</v>
       </c>
       <c r="B63">
-        <v>3116</v>
+        <v>3623</v>
       </c>
       <c r="E63">
         <v>2</v>
@@ -4082,13 +4271,16 @@
       <c r="Q63">
         <v>2881</v>
       </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R63">
+        <v>3116</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>43904</v>
       </c>
       <c r="B64">
-        <v>3361</v>
+        <v>3881</v>
       </c>
       <c r="E64">
         <v>0</v>
@@ -4129,13 +4321,16 @@
       <c r="Q64">
         <v>3026</v>
       </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R64">
+        <v>3361</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>43905</v>
       </c>
       <c r="B65">
-        <v>4077</v>
+        <v>4698</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -4176,13 +4371,16 @@
       <c r="Q65">
         <v>3688</v>
       </c>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R65">
+        <v>4077</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>43906</v>
       </c>
       <c r="B66">
-        <v>4662</v>
+        <v>5580</v>
       </c>
       <c r="G66">
         <v>2</v>
@@ -4217,13 +4415,16 @@
       <c r="Q66">
         <v>4150</v>
       </c>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R66">
+        <v>4662</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>43907</v>
       </c>
       <c r="B67">
-        <v>3965</v>
+        <v>4995</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -4258,13 +4459,16 @@
       <c r="Q67">
         <v>3456</v>
       </c>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R67">
+        <v>3965</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>43908</v>
       </c>
       <c r="B68">
-        <v>3809</v>
+        <v>4807</v>
       </c>
       <c r="G68">
         <v>0</v>
@@ -4299,13 +4503,16 @@
       <c r="Q68">
         <v>3270</v>
       </c>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R68">
+        <v>3809</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>43909</v>
       </c>
       <c r="B69">
-        <v>4345</v>
+        <v>5548</v>
       </c>
       <c r="H69">
         <v>0</v>
@@ -4337,13 +4544,16 @@
       <c r="Q69">
         <v>3899</v>
       </c>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R69">
+        <v>4345</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>43910</v>
       </c>
       <c r="B70">
-        <v>4588</v>
+        <v>5959</v>
       </c>
       <c r="I70">
         <v>2</v>
@@ -4372,13 +4582,16 @@
       <c r="Q70">
         <v>4024</v>
       </c>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R70">
+        <v>4588</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>43911</v>
       </c>
       <c r="B71">
-        <v>4475</v>
+        <v>5598</v>
       </c>
       <c r="J71">
         <v>2</v>
@@ -4404,13 +4617,16 @@
       <c r="Q71">
         <v>3793</v>
       </c>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R71">
+        <v>4475</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>43912</v>
       </c>
       <c r="B72">
-        <v>4280</v>
+        <v>5563</v>
       </c>
       <c r="J72">
         <v>1</v>
@@ -4436,13 +4652,16 @@
       <c r="Q72">
         <v>3327</v>
       </c>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A73" s="2">
+      <c r="R72">
+        <v>4280</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A73" s="3">
         <v>43913</v>
       </c>
       <c r="B73">
-        <v>3618</v>
+        <v>5449</v>
       </c>
       <c r="J73">
         <v>0</v>
@@ -4468,13 +4687,16 @@
       <c r="Q73">
         <v>2806</v>
       </c>
-    </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A74" s="2">
+      <c r="R73">
+        <v>3618</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A74" s="3">
         <v>43914</v>
       </c>
       <c r="B74">
-        <v>2375</v>
+        <v>3744</v>
       </c>
       <c r="K74">
         <v>0</v>
@@ -4497,13 +4719,16 @@
       <c r="Q74">
         <v>1809</v>
       </c>
-    </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A75" s="2">
+      <c r="R74">
+        <v>2375</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A75" s="3">
         <v>43915</v>
       </c>
       <c r="B75">
-        <v>1928</v>
+        <v>3261</v>
       </c>
       <c r="L75">
         <v>0</v>
@@ -4523,13 +4748,16 @@
       <c r="Q75">
         <v>1359</v>
       </c>
-    </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R75">
+        <v>1928</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>43916</v>
       </c>
       <c r="B76">
-        <v>2094</v>
+        <v>4314</v>
       </c>
       <c r="M76">
         <v>1</v>
@@ -4546,13 +4774,16 @@
       <c r="Q76">
         <v>1002</v>
       </c>
-    </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R76">
+        <v>2094</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>43917</v>
       </c>
       <c r="B77">
-        <v>1267</v>
+        <v>3545</v>
       </c>
       <c r="O77">
         <v>10</v>
@@ -4563,13 +4794,16 @@
       <c r="Q77">
         <v>487</v>
       </c>
-    </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R77">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>43918</v>
       </c>
       <c r="B78">
-        <v>436</v>
+        <v>2959</v>
       </c>
       <c r="O78">
         <v>2</v>
@@ -4580,13 +4814,16 @@
       <c r="Q78">
         <v>218</v>
       </c>
-    </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R78">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>43919</v>
       </c>
       <c r="B79">
-        <v>249</v>
+        <v>2066</v>
       </c>
       <c r="O79">
         <v>0</v>
@@ -4597,13 +4834,16 @@
       <c r="Q79">
         <v>119</v>
       </c>
-    </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R79">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>43920</v>
       </c>
       <c r="B80">
-        <v>146</v>
+        <v>1013</v>
       </c>
       <c r="P80">
         <v>3</v>
@@ -4611,13 +4851,16 @@
       <c r="Q80">
         <v>38</v>
       </c>
-    </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R80">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>43921</v>
       </c>
       <c r="B81">
-        <v>46</v>
+        <v>394</v>
       </c>
       <c r="P81">
         <v>0</v>
@@ -4625,23 +4868,64 @@
       <c r="Q81">
         <v>9</v>
       </c>
-    </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R81">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>43922</v>
       </c>
       <c r="B82">
-        <v>3</v>
+        <v>187</v>
       </c>
       <c r="Q82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R82">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>43923</v>
       </c>
       <c r="B83">
+        <v>72</v>
+      </c>
+      <c r="R83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>43924</v>
+      </c>
+      <c r="B84">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>43925</v>
+      </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>43926</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B87">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
14 apr cdc update
</commit_message>
<xml_diff>
--- a/data/CDC_data.xlsx
+++ b/data/CDC_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauernd\Documents\R\workspace\COVID-19_epi_info\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2253B6B5-1925-439C-A04A-FADF8B4A6B4D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B165457E-AAB2-44A9-A6CB-52AF91568F20}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="525" windowWidth="15720" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2025" yWindow="495" windowWidth="16485" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CDC_data_as_of_14_Mar" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>Date</t>
   </si>
@@ -886,7 +886,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B90"/>
+  <dimension ref="A1:B94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -924,7 +924,7 @@
         <v>43844</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -948,7 +948,7 @@
         <v>43847</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -988,7 +988,7 @@
         <v>43852</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -996,7 +996,7 @@
         <v>43853</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1004,7 +1004,7 @@
         <v>43854</v>
       </c>
       <c r="B14">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1012,7 +1012,7 @@
         <v>43855</v>
       </c>
       <c r="B15">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1020,7 +1020,7 @@
         <v>43856</v>
       </c>
       <c r="B16">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1028,7 +1028,7 @@
         <v>43857</v>
       </c>
       <c r="B17">
-        <v>17</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1060,7 +1060,7 @@
         <v>43861</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1068,7 +1068,7 @@
         <v>43862</v>
       </c>
       <c r="B22">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1076,7 +1076,7 @@
         <v>43863</v>
       </c>
       <c r="B23">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1084,7 +1084,7 @@
         <v>43864</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1092,7 +1092,7 @@
         <v>43865</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1108,7 +1108,7 @@
         <v>43867</v>
       </c>
       <c r="B27">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1116,7 +1116,7 @@
         <v>43868</v>
       </c>
       <c r="B28">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1132,7 +1132,7 @@
         <v>43870</v>
       </c>
       <c r="B30">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1156,7 +1156,7 @@
         <v>43873</v>
       </c>
       <c r="B33">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1172,7 +1172,7 @@
         <v>43875</v>
       </c>
       <c r="B35">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1180,7 +1180,7 @@
         <v>43876</v>
       </c>
       <c r="B36">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1188,7 +1188,7 @@
         <v>43877</v>
       </c>
       <c r="B37">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1204,7 +1204,7 @@
         <v>43879</v>
       </c>
       <c r="B39">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1220,7 +1220,7 @@
         <v>43881</v>
       </c>
       <c r="B41">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1228,7 +1228,7 @@
         <v>43882</v>
       </c>
       <c r="B42">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1236,7 +1236,7 @@
         <v>43883</v>
       </c>
       <c r="B43">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -1244,7 +1244,7 @@
         <v>43884</v>
       </c>
       <c r="B44">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1252,7 +1252,7 @@
         <v>43885</v>
       </c>
       <c r="B45">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1260,7 +1260,7 @@
         <v>43886</v>
       </c>
       <c r="B46">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1268,7 +1268,7 @@
         <v>43887</v>
       </c>
       <c r="B47">
-        <v>108</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1276,7 +1276,7 @@
         <v>43888</v>
       </c>
       <c r="B48">
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1284,7 +1284,7 @@
         <v>43889</v>
       </c>
       <c r="B49">
-        <v>170</v>
+        <v>181</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1292,7 +1292,7 @@
         <v>43890</v>
       </c>
       <c r="B50">
-        <v>141</v>
+        <v>160</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1300,7 +1300,7 @@
         <v>43891</v>
       </c>
       <c r="B51">
-        <v>342</v>
+        <v>374</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1308,7 +1308,7 @@
         <v>43892</v>
       </c>
       <c r="B52">
-        <v>330</v>
+        <v>366</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1316,7 +1316,7 @@
         <v>43893</v>
       </c>
       <c r="B53">
-        <v>385</v>
+        <v>421</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1324,7 +1324,7 @@
         <v>43894</v>
       </c>
       <c r="B54">
-        <v>428</v>
+        <v>466</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1332,7 +1332,7 @@
         <v>43895</v>
       </c>
       <c r="B55">
-        <v>514</v>
+        <v>547</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1340,7 +1340,7 @@
         <v>43896</v>
       </c>
       <c r="B56">
-        <v>676</v>
+        <v>730</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1348,7 +1348,7 @@
         <v>43897</v>
       </c>
       <c r="B57">
-        <v>833</v>
+        <v>872</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1356,7 +1356,7 @@
         <v>43898</v>
       </c>
       <c r="B58">
-        <v>1293</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -1364,7 +1364,7 @@
         <v>43899</v>
       </c>
       <c r="B59">
-        <v>2189</v>
+        <v>2325</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -1372,7 +1372,7 @@
         <v>43900</v>
       </c>
       <c r="B60">
-        <v>2350</v>
+        <v>2514</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -1380,7 +1380,7 @@
         <v>43901</v>
       </c>
       <c r="B61">
-        <v>3168</v>
+        <v>3327</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -1388,7 +1388,7 @@
         <v>43902</v>
       </c>
       <c r="B62">
-        <v>4997</v>
+        <v>5205</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1396,7 +1396,7 @@
         <v>43903</v>
       </c>
       <c r="B63">
-        <v>6243</v>
+        <v>6566</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1404,7 +1404,7 @@
         <v>43904</v>
       </c>
       <c r="B64">
-        <v>7063</v>
+        <v>7387</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1412,7 +1412,7 @@
         <v>43905</v>
       </c>
       <c r="B65">
-        <v>8595</v>
+        <v>9042</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -1420,7 +1420,7 @@
         <v>43906</v>
       </c>
       <c r="B66">
-        <v>10052</v>
+        <v>10675</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -1428,7 +1428,7 @@
         <v>43907</v>
       </c>
       <c r="B67">
-        <v>8211</v>
+        <v>8890</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -1436,7 +1436,7 @@
         <v>43908</v>
       </c>
       <c r="B68">
-        <v>8033</v>
+        <v>8733</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -1444,7 +1444,7 @@
         <v>43909</v>
       </c>
       <c r="B69">
-        <v>9741</v>
+        <v>10407</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1452,7 +1452,7 @@
         <v>43910</v>
       </c>
       <c r="B70">
-        <v>11572</v>
+        <v>12445</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1460,7 +1460,7 @@
         <v>43911</v>
       </c>
       <c r="B71">
-        <v>11755</v>
+        <v>12412</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -1468,7 +1468,7 @@
         <v>43912</v>
       </c>
       <c r="B72">
-        <v>12214</v>
+        <v>12817</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -1476,7 +1476,7 @@
         <v>43913</v>
       </c>
       <c r="B73">
-        <v>13194</v>
+        <v>14190</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -1484,7 +1484,7 @@
         <v>43914</v>
       </c>
       <c r="B74">
-        <v>9476</v>
+        <v>10272</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -1492,7 +1492,7 @@
         <v>43915</v>
       </c>
       <c r="B75">
-        <v>9669</v>
+        <v>10545</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -1500,7 +1500,7 @@
         <v>43916</v>
       </c>
       <c r="B76">
-        <v>14491</v>
+        <v>15451</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -1508,7 +1508,7 @@
         <v>43917</v>
       </c>
       <c r="B77">
-        <v>13350</v>
+        <v>14728</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -1516,7 +1516,7 @@
         <v>43918</v>
       </c>
       <c r="B78">
-        <v>12673</v>
+        <v>14088</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1524,39 +1524,39 @@
         <v>43919</v>
       </c>
       <c r="B79">
-        <v>12967</v>
+        <v>14092</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="2">
+      <c r="A80" s="3">
         <v>43920</v>
       </c>
       <c r="B80">
-        <v>13223</v>
+        <v>14651</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="2">
+      <c r="A81" s="3">
         <v>43921</v>
       </c>
       <c r="B81">
-        <v>9331</v>
+        <v>10849</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="2">
+      <c r="A82" s="3">
         <v>43922</v>
       </c>
       <c r="B82">
-        <v>8569</v>
+        <v>10194</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="2">
+      <c r="A83" s="3">
         <v>43923</v>
       </c>
       <c r="B83">
-        <v>11529</v>
+        <v>15451</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -1564,7 +1564,7 @@
         <v>43924</v>
       </c>
       <c r="B84">
-        <v>8136</v>
+        <v>14774</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -1572,7 +1572,7 @@
         <v>43925</v>
       </c>
       <c r="B85">
-        <v>4155</v>
+        <v>12417</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -1580,7 +1580,7 @@
         <v>43926</v>
       </c>
       <c r="B86">
-        <v>1116</v>
+        <v>9328</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -1588,7 +1588,7 @@
         <v>43927</v>
       </c>
       <c r="B87">
-        <v>434</v>
+        <v>7911</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -1596,7 +1596,7 @@
         <v>43928</v>
       </c>
       <c r="B88">
-        <v>151</v>
+        <v>3525</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -1604,7 +1604,7 @@
         <v>43929</v>
       </c>
       <c r="B89">
-        <v>47</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -1612,7 +1612,39 @@
         <v>43930</v>
       </c>
       <c r="B90">
-        <v>11</v>
+        <v>365</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>43931</v>
+      </c>
+      <c r="B91">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <v>43932</v>
+      </c>
+      <c r="B92">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B93">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
+        <v>43934</v>
+      </c>
+      <c r="B94">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with cdc 15 apr data
</commit_message>
<xml_diff>
--- a/data/CDC_data.xlsx
+++ b/data/CDC_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauernd\Documents\R\workspace\COVID-19_epi_info\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B165457E-AAB2-44A9-A6CB-52AF91568F20}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CF6016-7467-4F7F-8882-2E0F79EC1A5D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2025" yWindow="495" windowWidth="16485" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="315" windowWidth="15720" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CDC_data_as_of_14_Mar" sheetId="1" r:id="rId1"/>
@@ -886,9 +886,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B94"/>
+  <dimension ref="A1:B95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1108,7 +1110,7 @@
         <v>43867</v>
       </c>
       <c r="B27">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1132,7 +1134,7 @@
         <v>43870</v>
       </c>
       <c r="B30">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1140,7 +1142,7 @@
         <v>43871</v>
       </c>
       <c r="B31">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1164,7 +1166,7 @@
         <v>43874</v>
       </c>
       <c r="B34">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1188,7 +1190,7 @@
         <v>43877</v>
       </c>
       <c r="B37">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1196,7 +1198,7 @@
         <v>43878</v>
       </c>
       <c r="B38">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1212,7 +1214,7 @@
         <v>43880</v>
       </c>
       <c r="B40">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1228,7 +1230,7 @@
         <v>43882</v>
       </c>
       <c r="B42">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1252,7 +1254,7 @@
         <v>43885</v>
       </c>
       <c r="B45">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1260,7 +1262,7 @@
         <v>43886</v>
       </c>
       <c r="B46">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1268,7 +1270,7 @@
         <v>43887</v>
       </c>
       <c r="B47">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1276,7 +1278,7 @@
         <v>43888</v>
       </c>
       <c r="B48">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1284,7 +1286,7 @@
         <v>43889</v>
       </c>
       <c r="B49">
-        <v>181</v>
+        <v>188</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1292,7 +1294,7 @@
         <v>43890</v>
       </c>
       <c r="B50">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1300,7 +1302,7 @@
         <v>43891</v>
       </c>
       <c r="B51">
-        <v>374</v>
+        <v>385</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1308,7 +1310,7 @@
         <v>43892</v>
       </c>
       <c r="B52">
-        <v>366</v>
+        <v>370</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1316,7 +1318,7 @@
         <v>43893</v>
       </c>
       <c r="B53">
-        <v>421</v>
+        <v>426</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1324,7 +1326,7 @@
         <v>43894</v>
       </c>
       <c r="B54">
-        <v>466</v>
+        <v>471</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1332,7 +1334,7 @@
         <v>43895</v>
       </c>
       <c r="B55">
-        <v>547</v>
+        <v>553</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1340,7 +1342,7 @@
         <v>43896</v>
       </c>
       <c r="B56">
-        <v>730</v>
+        <v>735</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1348,7 +1350,7 @@
         <v>43897</v>
       </c>
       <c r="B57">
-        <v>872</v>
+        <v>883</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1356,7 +1358,7 @@
         <v>43898</v>
       </c>
       <c r="B58">
-        <v>1377</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -1364,7 +1366,7 @@
         <v>43899</v>
       </c>
       <c r="B59">
-        <v>2325</v>
+        <v>2355</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -1372,7 +1374,7 @@
         <v>43900</v>
       </c>
       <c r="B60">
-        <v>2514</v>
+        <v>2538</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -1380,7 +1382,7 @@
         <v>43901</v>
       </c>
       <c r="B61">
-        <v>3327</v>
+        <v>3358</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -1388,7 +1390,7 @@
         <v>43902</v>
       </c>
       <c r="B62">
-        <v>5205</v>
+        <v>5254</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1396,7 +1398,7 @@
         <v>43903</v>
       </c>
       <c r="B63">
-        <v>6566</v>
+        <v>6606</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1404,7 +1406,7 @@
         <v>43904</v>
       </c>
       <c r="B64">
-        <v>7387</v>
+        <v>7438</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1412,7 +1414,7 @@
         <v>43905</v>
       </c>
       <c r="B65">
-        <v>9042</v>
+        <v>9100</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -1420,7 +1422,7 @@
         <v>43906</v>
       </c>
       <c r="B66">
-        <v>10675</v>
+        <v>10742</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -1428,7 +1430,7 @@
         <v>43907</v>
       </c>
       <c r="B67">
-        <v>8890</v>
+        <v>8945</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -1436,7 +1438,7 @@
         <v>43908</v>
       </c>
       <c r="B68">
-        <v>8733</v>
+        <v>8790</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -1444,7 +1446,7 @@
         <v>43909</v>
       </c>
       <c r="B69">
-        <v>10407</v>
+        <v>10483</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1452,7 +1454,7 @@
         <v>43910</v>
       </c>
       <c r="B70">
-        <v>12445</v>
+        <v>12509</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1460,7 +1462,7 @@
         <v>43911</v>
       </c>
       <c r="B71">
-        <v>12412</v>
+        <v>12365</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -1476,7 +1478,7 @@
         <v>43913</v>
       </c>
       <c r="B73">
-        <v>14190</v>
+        <v>14306</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -1484,7 +1486,7 @@
         <v>43914</v>
       </c>
       <c r="B74">
-        <v>10272</v>
+        <v>10409</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -1492,7 +1494,7 @@
         <v>43915</v>
       </c>
       <c r="B75">
-        <v>10545</v>
+        <v>10661</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -1500,7 +1502,7 @@
         <v>43916</v>
       </c>
       <c r="B76">
-        <v>15451</v>
+        <v>15546</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -1508,7 +1510,7 @@
         <v>43917</v>
       </c>
       <c r="B77">
-        <v>14728</v>
+        <v>14804</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -1516,7 +1518,7 @@
         <v>43918</v>
       </c>
       <c r="B78">
-        <v>14088</v>
+        <v>14256</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1524,7 +1526,7 @@
         <v>43919</v>
       </c>
       <c r="B79">
-        <v>14092</v>
+        <v>14305</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -1532,7 +1534,7 @@
         <v>43920</v>
       </c>
       <c r="B80">
-        <v>14651</v>
+        <v>14976</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -1540,7 +1542,7 @@
         <v>43921</v>
       </c>
       <c r="B81">
-        <v>10849</v>
+        <v>11096</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -1548,7 +1550,7 @@
         <v>43922</v>
       </c>
       <c r="B82">
-        <v>10194</v>
+        <v>10479</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -1556,15 +1558,15 @@
         <v>43923</v>
       </c>
       <c r="B83">
-        <v>15451</v>
+        <v>15666</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="2">
+      <c r="A84" s="3">
         <v>43924</v>
       </c>
       <c r="B84">
-        <v>14774</v>
+        <v>15052</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -1572,7 +1574,7 @@
         <v>43925</v>
       </c>
       <c r="B85">
-        <v>12417</v>
+        <v>13384</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -1580,7 +1582,7 @@
         <v>43926</v>
       </c>
       <c r="B86">
-        <v>9328</v>
+        <v>11014</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -1588,7 +1590,7 @@
         <v>43927</v>
       </c>
       <c r="B87">
-        <v>7911</v>
+        <v>9952</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -1596,7 +1598,7 @@
         <v>43928</v>
       </c>
       <c r="B88">
-        <v>3525</v>
+        <v>5271</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -1604,7 +1606,7 @@
         <v>43929</v>
       </c>
       <c r="B89">
-        <v>1232</v>
+        <v>2894</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -1612,7 +1614,7 @@
         <v>43930</v>
       </c>
       <c r="B90">
-        <v>365</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -1620,7 +1622,7 @@
         <v>43931</v>
       </c>
       <c r="B91">
-        <v>144</v>
+        <v>386</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -1628,7 +1630,7 @@
         <v>43932</v>
       </c>
       <c r="B92">
-        <v>27</v>
+        <v>126</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -1636,7 +1638,7 @@
         <v>43933</v>
       </c>
       <c r="B93">
-        <v>9</v>
+        <v>56</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -1644,7 +1646,15 @@
         <v>43934</v>
       </c>
       <c r="B94">
-        <v>0</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B95">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with 16 apr cdc date corrected error in gr calculations
</commit_message>
<xml_diff>
--- a/data/CDC_data.xlsx
+++ b/data/CDC_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauernd\Documents\R\workspace\COVID-19_epi_info\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CF6016-7467-4F7F-8882-2E0F79EC1A5D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE656D78-09B7-4142-9E1F-FAAC571118BB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="315" windowWidth="15720" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="375" windowWidth="21945" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CDC_data_as_of_14_Mar" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Date</t>
   </si>
@@ -886,10 +886,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B95"/>
+  <dimension ref="A1:B96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,7 +950,7 @@
         <v>43847</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -958,7 +958,7 @@
         <v>43848</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -966,7 +966,7 @@
         <v>43849</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -974,7 +974,7 @@
         <v>43850</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -982,7 +982,7 @@
         <v>43851</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1038,7 +1038,7 @@
         <v>43858</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1054,7 +1054,7 @@
         <v>43860</v>
       </c>
       <c r="B20">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1070,7 +1070,7 @@
         <v>43862</v>
       </c>
       <c r="B22">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1078,7 +1078,7 @@
         <v>43863</v>
       </c>
       <c r="B23">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1086,7 +1086,7 @@
         <v>43864</v>
       </c>
       <c r="B24">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1102,7 +1102,7 @@
         <v>43866</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1126,7 +1126,7 @@
         <v>43869</v>
       </c>
       <c r="B29">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1134,7 +1134,7 @@
         <v>43870</v>
       </c>
       <c r="B30">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1158,7 +1158,7 @@
         <v>43873</v>
       </c>
       <c r="B33">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1174,7 +1174,7 @@
         <v>43875</v>
       </c>
       <c r="B35">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1182,7 +1182,7 @@
         <v>43876</v>
       </c>
       <c r="B36">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1190,7 +1190,7 @@
         <v>43877</v>
       </c>
       <c r="B37">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1206,7 +1206,7 @@
         <v>43879</v>
       </c>
       <c r="B39">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1214,7 +1214,7 @@
         <v>43880</v>
       </c>
       <c r="B40">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1222,7 +1222,7 @@
         <v>43881</v>
       </c>
       <c r="B41">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1230,7 +1230,7 @@
         <v>43882</v>
       </c>
       <c r="B42">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1238,7 +1238,7 @@
         <v>43883</v>
       </c>
       <c r="B43">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -1246,7 +1246,7 @@
         <v>43884</v>
       </c>
       <c r="B44">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1254,7 +1254,7 @@
         <v>43885</v>
       </c>
       <c r="B45">
-        <v>101</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1262,7 +1262,7 @@
         <v>43886</v>
       </c>
       <c r="B46">
-        <v>81</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1270,7 +1270,7 @@
         <v>43887</v>
       </c>
       <c r="B47">
-        <v>119</v>
+        <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1278,7 +1278,7 @@
         <v>43888</v>
       </c>
       <c r="B48">
-        <v>118</v>
+        <v>128</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1286,7 +1286,7 @@
         <v>43889</v>
       </c>
       <c r="B49">
-        <v>188</v>
+        <v>207</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1294,7 +1294,7 @@
         <v>43890</v>
       </c>
       <c r="B50">
-        <v>162</v>
+        <v>170</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1302,7 +1302,7 @@
         <v>43891</v>
       </c>
       <c r="B51">
-        <v>385</v>
+        <v>441</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1310,7 +1310,7 @@
         <v>43892</v>
       </c>
       <c r="B52">
-        <v>370</v>
+        <v>413</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1318,7 +1318,7 @@
         <v>43893</v>
       </c>
       <c r="B53">
-        <v>426</v>
+        <v>466</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1326,7 +1326,7 @@
         <v>43894</v>
       </c>
       <c r="B54">
-        <v>471</v>
+        <v>530</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1334,7 +1334,7 @@
         <v>43895</v>
       </c>
       <c r="B55">
-        <v>553</v>
+        <v>600</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1342,7 +1342,7 @@
         <v>43896</v>
       </c>
       <c r="B56">
-        <v>735</v>
+        <v>794</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1350,7 +1350,7 @@
         <v>43897</v>
       </c>
       <c r="B57">
-        <v>883</v>
+        <v>946</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1358,7 +1358,7 @@
         <v>43898</v>
       </c>
       <c r="B58">
-        <v>1397</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -1366,7 +1366,7 @@
         <v>43899</v>
       </c>
       <c r="B59">
-        <v>2355</v>
+        <v>2505</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -1374,7 +1374,7 @@
         <v>43900</v>
       </c>
       <c r="B60">
-        <v>2538</v>
+        <v>2739</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -1382,7 +1382,7 @@
         <v>43901</v>
       </c>
       <c r="B61">
-        <v>3358</v>
+        <v>3543</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -1390,7 +1390,7 @@
         <v>43902</v>
       </c>
       <c r="B62">
-        <v>5254</v>
+        <v>5480</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1398,7 +1398,7 @@
         <v>43903</v>
       </c>
       <c r="B63">
-        <v>6606</v>
+        <v>6916</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1406,7 +1406,7 @@
         <v>43904</v>
       </c>
       <c r="B64">
-        <v>7438</v>
+        <v>7818</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1414,7 +1414,7 @@
         <v>43905</v>
       </c>
       <c r="B65">
-        <v>9100</v>
+        <v>9496</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -1422,7 +1422,7 @@
         <v>43906</v>
       </c>
       <c r="B66">
-        <v>10742</v>
+        <v>11381</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -1430,7 +1430,7 @@
         <v>43907</v>
       </c>
       <c r="B67">
-        <v>8945</v>
+        <v>9497</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -1438,7 +1438,7 @@
         <v>43908</v>
       </c>
       <c r="B68">
-        <v>8790</v>
+        <v>9431</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -1446,7 +1446,7 @@
         <v>43909</v>
       </c>
       <c r="B69">
-        <v>10483</v>
+        <v>11087</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1454,7 +1454,7 @@
         <v>43910</v>
       </c>
       <c r="B70">
-        <v>12509</v>
+        <v>13231</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1462,7 +1462,7 @@
         <v>43911</v>
       </c>
       <c r="B71">
-        <v>12365</v>
+        <v>13020</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -1470,7 +1470,7 @@
         <v>43912</v>
       </c>
       <c r="B72">
-        <v>12817</v>
+        <v>13477</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -1478,7 +1478,7 @@
         <v>43913</v>
       </c>
       <c r="B73">
-        <v>14306</v>
+        <v>15208</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -1486,7 +1486,7 @@
         <v>43914</v>
       </c>
       <c r="B74">
-        <v>10409</v>
+        <v>11117</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -1494,7 +1494,7 @@
         <v>43915</v>
       </c>
       <c r="B75">
-        <v>10661</v>
+        <v>11505</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -1502,7 +1502,7 @@
         <v>43916</v>
       </c>
       <c r="B76">
-        <v>15546</v>
+        <v>16287</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -1510,7 +1510,7 @@
         <v>43917</v>
       </c>
       <c r="B77">
-        <v>14804</v>
+        <v>15455</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -1518,7 +1518,7 @@
         <v>43918</v>
       </c>
       <c r="B78">
-        <v>14256</v>
+        <v>14855</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1526,7 +1526,7 @@
         <v>43919</v>
       </c>
       <c r="B79">
-        <v>14305</v>
+        <v>14753</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -1534,7 +1534,7 @@
         <v>43920</v>
       </c>
       <c r="B80">
-        <v>14976</v>
+        <v>15942</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -1542,7 +1542,7 @@
         <v>43921</v>
       </c>
       <c r="B81">
-        <v>11096</v>
+        <v>11648</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -1550,7 +1550,7 @@
         <v>43922</v>
       </c>
       <c r="B82">
-        <v>10479</v>
+        <v>11219</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -1558,7 +1558,7 @@
         <v>43923</v>
       </c>
       <c r="B83">
-        <v>15666</v>
+        <v>16092</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -1566,15 +1566,15 @@
         <v>43924</v>
       </c>
       <c r="B84">
-        <v>15052</v>
+        <v>15618</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="2">
+      <c r="A85" s="3">
         <v>43925</v>
       </c>
       <c r="B85">
-        <v>13384</v>
+        <v>13968</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -1582,7 +1582,7 @@
         <v>43926</v>
       </c>
       <c r="B86">
-        <v>11014</v>
+        <v>11663</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -1590,7 +1590,7 @@
         <v>43927</v>
       </c>
       <c r="B87">
-        <v>9952</v>
+        <v>10886</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -1598,7 +1598,7 @@
         <v>43928</v>
       </c>
       <c r="B88">
-        <v>5271</v>
+        <v>6183</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -1606,7 +1606,7 @@
         <v>43929</v>
       </c>
       <c r="B89">
-        <v>2894</v>
+        <v>4176</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -1614,7 +1614,7 @@
         <v>43930</v>
       </c>
       <c r="B90">
-        <v>1606</v>
+        <v>4177</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -1622,7 +1622,7 @@
         <v>43931</v>
       </c>
       <c r="B91">
-        <v>386</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -1630,7 +1630,7 @@
         <v>43932</v>
       </c>
       <c r="B92">
-        <v>126</v>
+        <v>339</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -1638,7 +1638,7 @@
         <v>43933</v>
       </c>
       <c r="B93">
-        <v>56</v>
+        <v>182</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -1646,7 +1646,7 @@
         <v>43934</v>
       </c>
       <c r="B94">
-        <v>13</v>
+        <v>102</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -1654,7 +1654,15 @@
         <v>43935</v>
       </c>
       <c r="B95">
-        <v>2</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
+        <v>43936</v>
+      </c>
+      <c r="B96">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New CDC data 11 May
</commit_message>
<xml_diff>
--- a/data/CDC_data.xlsx
+++ b/data/CDC_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauernd\Documents\R\workspace\COVID-19_epi_info\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE656D78-09B7-4142-9E1F-FAAC571118BB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A8EE58-1390-4ADF-82EA-CC1539D9C174}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="375" windowWidth="21945" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="540" windowWidth="18240" windowHeight="9330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CDC_data_as_of_14_Mar" sheetId="1" r:id="rId1"/>
@@ -28,12 +28,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Date</t>
   </si>
   <si>
     <t>cases</t>
+  </si>
+  <si>
+    <t>cases old</t>
   </si>
 </sst>
 </file>
@@ -179,7 +182,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -357,12 +360,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -526,10 +523,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -886,10 +881,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B96"/>
+  <dimension ref="A1:C122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,772 +892,1265 @@
     <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43842</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43843</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43844</v>
       </c>
       <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43845</v>
       </c>
       <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43846</v>
       </c>
       <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43847</v>
       </c>
       <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43848</v>
       </c>
       <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43849</v>
       </c>
       <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43850</v>
       </c>
       <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43851</v>
       </c>
       <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43852</v>
       </c>
       <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43853</v>
       </c>
       <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43854</v>
       </c>
       <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43855</v>
       </c>
       <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43856</v>
       </c>
       <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43857</v>
       </c>
       <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43858</v>
       </c>
       <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43859</v>
       </c>
       <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43860</v>
       </c>
       <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43861</v>
       </c>
       <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43862</v>
       </c>
       <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43863</v>
       </c>
       <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43864</v>
       </c>
       <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43865</v>
       </c>
       <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43866</v>
       </c>
       <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43867</v>
       </c>
       <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43868</v>
       </c>
       <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43869</v>
       </c>
       <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43870</v>
       </c>
       <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43871</v>
       </c>
       <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>43872</v>
       </c>
       <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43873</v>
       </c>
       <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43874</v>
       </c>
       <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43875</v>
       </c>
       <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43876</v>
       </c>
       <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43877</v>
       </c>
       <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>43878</v>
       </c>
       <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>43879</v>
       </c>
       <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>43880</v>
       </c>
       <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>43881</v>
       </c>
       <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>43882</v>
       </c>
       <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42">
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43883</v>
       </c>
       <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43884</v>
       </c>
       <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43885</v>
       </c>
       <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
         <v>109</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>43886</v>
       </c>
       <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
         <v>92</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>43887</v>
       </c>
       <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
         <v>126</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>43888</v>
       </c>
       <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
         <v>128</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>43889</v>
       </c>
       <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
         <v>207</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>43890</v>
       </c>
       <c r="B50">
+        <v>8</v>
+      </c>
+      <c r="C50">
         <v>170</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>43891</v>
       </c>
       <c r="B51">
+        <v>6</v>
+      </c>
+      <c r="C51">
         <v>441</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>43892</v>
       </c>
       <c r="B52">
+        <v>23</v>
+      </c>
+      <c r="C52">
         <v>413</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>43893</v>
       </c>
       <c r="B53">
+        <v>25</v>
+      </c>
+      <c r="C53">
         <v>466</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>43894</v>
       </c>
       <c r="B54">
+        <v>20</v>
+      </c>
+      <c r="C54">
         <v>530</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>43895</v>
       </c>
       <c r="B55">
+        <v>66</v>
+      </c>
+      <c r="C55">
         <v>600</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>43896</v>
       </c>
       <c r="B56">
+        <v>47</v>
+      </c>
+      <c r="C56">
         <v>794</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>43897</v>
       </c>
       <c r="B57">
+        <v>64</v>
+      </c>
+      <c r="C57">
         <v>946</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>43898</v>
       </c>
       <c r="B58">
+        <v>147</v>
+      </c>
+      <c r="C58">
         <v>1470</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>43899</v>
       </c>
       <c r="B59">
+        <v>225</v>
+      </c>
+      <c r="C59">
         <v>2505</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>43900</v>
       </c>
       <c r="B60">
+        <v>290</v>
+      </c>
+      <c r="C60">
         <v>2739</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>43901</v>
       </c>
       <c r="B61">
+        <v>278</v>
+      </c>
+      <c r="C61">
         <v>3543</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>43902</v>
       </c>
       <c r="B62">
+        <v>414</v>
+      </c>
+      <c r="C62">
         <v>5480</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>43903</v>
       </c>
       <c r="B63">
+        <v>267</v>
+      </c>
+      <c r="C63">
         <v>6916</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>43904</v>
       </c>
       <c r="B64">
+        <v>338</v>
+      </c>
+      <c r="C64">
         <v>7818</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
         <v>43905</v>
       </c>
       <c r="B65">
+        <v>1237</v>
+      </c>
+      <c r="C65">
         <v>9496</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
         <v>43906</v>
       </c>
       <c r="B66">
+        <v>755</v>
+      </c>
+      <c r="C66">
         <v>11381</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
         <v>43907</v>
       </c>
       <c r="B67">
+        <v>2797</v>
+      </c>
+      <c r="C67">
         <v>9497</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
         <v>43908</v>
       </c>
       <c r="B68">
+        <v>3419</v>
+      </c>
+      <c r="C68">
         <v>9431</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
         <v>43909</v>
       </c>
       <c r="B69">
+        <v>4777</v>
+      </c>
+      <c r="C69">
         <v>11087</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
         <v>43910</v>
       </c>
       <c r="B70">
+        <v>3528</v>
+      </c>
+      <c r="C70">
         <v>13231</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
         <v>43911</v>
       </c>
       <c r="B71">
+        <v>5836</v>
+      </c>
+      <c r="C71">
         <v>13020</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
         <v>43912</v>
       </c>
       <c r="B72">
+        <v>8821</v>
+      </c>
+      <c r="C72">
         <v>13477</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
         <v>43913</v>
       </c>
       <c r="B73">
+        <v>10934</v>
+      </c>
+      <c r="C73">
         <v>15208</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
         <v>43914</v>
       </c>
       <c r="B74">
+        <v>10115</v>
+      </c>
+      <c r="C74">
         <v>11117</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
         <v>43915</v>
       </c>
       <c r="B75">
+        <v>13987</v>
+      </c>
+      <c r="C75">
         <v>11505</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
         <v>43916</v>
       </c>
       <c r="B76">
+        <v>16916</v>
+      </c>
+      <c r="C76">
         <v>16287</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
         <v>43917</v>
       </c>
       <c r="B77">
+        <v>17965</v>
+      </c>
+      <c r="C77">
         <v>15455</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
         <v>43918</v>
       </c>
       <c r="B78">
+        <v>19332</v>
+      </c>
+      <c r="C78">
         <v>14855</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
         <v>43919</v>
       </c>
       <c r="B79">
+        <v>18251</v>
+      </c>
+      <c r="C79">
         <v>14753</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
         <v>43920</v>
       </c>
       <c r="B80">
+        <v>22635</v>
+      </c>
+      <c r="C80">
         <v>15942</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
         <v>43921</v>
       </c>
       <c r="B81">
+        <v>22562</v>
+      </c>
+      <c r="C81">
         <v>11648</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
         <v>43922</v>
       </c>
       <c r="B82">
+        <v>27043</v>
+      </c>
+      <c r="C82">
         <v>11219</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
         <v>43923</v>
       </c>
       <c r="B83">
+        <v>26135</v>
+      </c>
+      <c r="C83">
         <v>16092</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
         <v>43924</v>
       </c>
       <c r="B84">
+        <v>34864</v>
+      </c>
+      <c r="C84">
         <v>15618</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
         <v>43925</v>
       </c>
       <c r="B85">
+        <v>30683</v>
+      </c>
+      <c r="C85">
         <v>13968</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
         <v>43926</v>
       </c>
       <c r="B86">
+        <v>26065</v>
+      </c>
+      <c r="C86">
         <v>11663</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="2">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
         <v>43927</v>
       </c>
       <c r="B87">
+        <v>43438</v>
+      </c>
+      <c r="C87">
         <v>10886</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
         <v>43928</v>
       </c>
       <c r="B88">
+        <v>20682</v>
+      </c>
+      <c r="C88">
         <v>6183</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
         <v>43929</v>
       </c>
       <c r="B89">
+        <v>32449</v>
+      </c>
+      <c r="C89">
         <v>4176</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="2">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
         <v>43930</v>
       </c>
       <c r="B90">
+        <v>31705</v>
+      </c>
+      <c r="C90">
         <v>4177</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="2">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
         <v>43931</v>
       </c>
       <c r="B91">
+        <v>33251</v>
+      </c>
+      <c r="C91">
         <v>1363</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="2">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
         <v>43932</v>
       </c>
       <c r="B92">
+        <v>33288</v>
+      </c>
+      <c r="C92">
         <v>339</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="2">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
         <v>43933</v>
       </c>
       <c r="B93">
+        <v>29145</v>
+      </c>
+      <c r="C93">
         <v>182</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="2">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
         <v>43934</v>
       </c>
       <c r="B94">
+        <v>24242</v>
+      </c>
+      <c r="C94">
         <v>102</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="2">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
         <v>43935</v>
       </c>
       <c r="B95">
+        <v>26527</v>
+      </c>
+      <c r="C95">
         <v>19</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="2">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
         <v>43936</v>
       </c>
       <c r="B96">
-        <v>0</v>
+        <v>26930</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>43937</v>
+      </c>
+      <c r="B97">
+        <v>29164</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>43938</v>
+      </c>
+      <c r="B98">
+        <v>29836</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>43939</v>
+      </c>
+      <c r="B99">
+        <v>29895</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>43940</v>
+      </c>
+      <c r="B100">
+        <v>26543</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>43941</v>
+      </c>
+      <c r="B101">
+        <v>29468</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>43942</v>
+      </c>
+      <c r="B102">
+        <v>26490</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>43943</v>
+      </c>
+      <c r="B103">
+        <v>25858</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>43944</v>
+      </c>
+      <c r="B104">
+        <v>37144</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>43945</v>
+      </c>
+      <c r="B105">
+        <v>30181</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>43946</v>
+      </c>
+      <c r="B106">
+        <v>32853</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>43947</v>
+      </c>
+      <c r="B107">
+        <v>29256</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <v>43948</v>
+      </c>
+      <c r="B108">
+        <v>23371</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>43949</v>
+      </c>
+      <c r="B109">
+        <v>23901</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>43950</v>
+      </c>
+      <c r="B110">
+        <v>25512</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>43951</v>
+      </c>
+      <c r="B111">
+        <v>31787</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <v>43952</v>
+      </c>
+      <c r="B112">
+        <v>30269</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <v>43953</v>
+      </c>
+      <c r="B113">
+        <v>29794</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>43954</v>
+      </c>
+      <c r="B114">
+        <v>29763</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>43955</v>
+      </c>
+      <c r="B115">
+        <v>19138</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <v>43956</v>
+      </c>
+      <c r="B116">
+        <v>22303</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
+        <v>43957</v>
+      </c>
+      <c r="B117">
+        <v>25253</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <v>43958</v>
+      </c>
+      <c r="B118">
+        <v>28974</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <v>43959</v>
+      </c>
+      <c r="B119">
+        <v>25996</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>43960</v>
+      </c>
+      <c r="B120">
+        <v>26660</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <v>43961</v>
+      </c>
+      <c r="B121">
+        <v>23792</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="1">
+        <v>43962</v>
       </c>
     </row>
   </sheetData>

</xml_diff>